<commit_message>
2022 07 31 pagi
</commit_message>
<xml_diff>
--- a/assets/apriori baru.xlsx
+++ b/assets/apriori baru.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\201753028\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -403,7 +403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3938,8 +3938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:L32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2022 08 05 06:10
</commit_message>
<xml_diff>
--- a/assets/apriori baru.xlsx
+++ b/assets/apriori baru.xlsx
@@ -9,13 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="contoh 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="percobaan" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
   <si>
     <t>Data</t>
   </si>
@@ -398,13 +403,85 @@
   </si>
   <si>
     <t>Aturan yang didapat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username </t>
+  </si>
+  <si>
+    <t>yusuf_hidayat</t>
+  </si>
+  <si>
+    <t>$tr2    = [$barang0, $barang2, $barang3, $barang4];</t>
+  </si>
+  <si>
+    <t>$tr1    = [$barang0, $barang1, $barang2, $barang3];</t>
+  </si>
+  <si>
+    <t>$tr3    = [$barang0, $barang4, $barang5];</t>
+  </si>
+  <si>
+    <t>$tr4    = [$barang0, $barang1, $barang2, $barang4];</t>
+  </si>
+  <si>
+    <t>$tr5    = [$barang0, $barang1, $barang2, $barang3, $barang5];</t>
+  </si>
+  <si>
+    <t>$tr6    = [$barang0, $barang1, $barang2, $barang3, $barang4];</t>
+  </si>
+  <si>
+    <t>checkout1</t>
+  </si>
+  <si>
+    <t>checkout2</t>
+  </si>
+  <si>
+    <t>checkout3</t>
+  </si>
+  <si>
+    <t>checkout4</t>
+  </si>
+  <si>
+    <t>checkout5</t>
+  </si>
+  <si>
+    <t>checkout6</t>
+  </si>
+  <si>
+    <t>checkout = [ id_produk ]</t>
+  </si>
+  <si>
+    <t>SQL INSERT</t>
+  </si>
+  <si>
+    <t>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ('[value-1]','[value-2]','[value-3]','[value-4]','[value-5]','[value-6]')</t>
+  </si>
+  <si>
+    <t>id_keranjang</t>
+  </si>
+  <si>
+    <t>id_produk</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>jumlah_keranjang</t>
+  </si>
+  <si>
+    <t>harga_keranjang</t>
+  </si>
+  <si>
+    <t>status_keranjang</t>
+  </si>
+  <si>
+    <t>keranjang1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +502,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +525,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +737,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3671,6 +3770,1513 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="bank"/>
+      <sheetName val="Sheet7"/>
+      <sheetName val="gerai"/>
+      <sheetName val="user"/>
+      <sheetName val="stok_gerai"/>
+      <sheetName val="Sheet6"/>
+      <sheetName val="clear"/>
+      <sheetName val="produk"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
+        <row r="2">
+          <cell r="A2">
+            <v>2</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+          <cell r="D2">
+            <v>20</v>
+          </cell>
+          <cell r="E2">
+            <v>1</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G2" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="H2">
+            <v>20000</v>
+          </cell>
+          <cell r="I2">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>3</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="C3">
+            <v>2</v>
+          </cell>
+          <cell r="D3">
+            <v>20</v>
+          </cell>
+          <cell r="E3">
+            <v>1</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="H3">
+            <v>30000</v>
+          </cell>
+          <cell r="I3">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>4</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="C4">
+            <v>3</v>
+          </cell>
+          <cell r="D4">
+            <v>20</v>
+          </cell>
+          <cell r="E4">
+            <v>1</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G4" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="H4">
+            <v>40000</v>
+          </cell>
+          <cell r="I4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>5</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="C5">
+            <v>4</v>
+          </cell>
+          <cell r="D5">
+            <v>20</v>
+          </cell>
+          <cell r="E5">
+            <v>1</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="H5">
+            <v>50000</v>
+          </cell>
+          <cell r="I5">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>6</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="C6">
+            <v>5</v>
+          </cell>
+          <cell r="D6">
+            <v>20</v>
+          </cell>
+          <cell r="E6">
+            <v>1</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G6" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="H6">
+            <v>60000</v>
+          </cell>
+          <cell r="I6">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>7</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="C7">
+            <v>1</v>
+          </cell>
+          <cell r="D7">
+            <v>20</v>
+          </cell>
+          <cell r="E7">
+            <v>1</v>
+          </cell>
+          <cell r="F7" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G7" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="H7">
+            <v>70000</v>
+          </cell>
+          <cell r="I7">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>8</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="C8">
+            <v>2</v>
+          </cell>
+          <cell r="D8">
+            <v>20</v>
+          </cell>
+          <cell r="E8">
+            <v>1</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G8" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="H8">
+            <v>80000</v>
+          </cell>
+          <cell r="I8">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>9</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="C9">
+            <v>3</v>
+          </cell>
+          <cell r="D9">
+            <v>20</v>
+          </cell>
+          <cell r="E9">
+            <v>1</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G9" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="H9">
+            <v>90000</v>
+          </cell>
+          <cell r="I9">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>10</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="C10">
+            <v>4</v>
+          </cell>
+          <cell r="D10">
+            <v>20</v>
+          </cell>
+          <cell r="E10">
+            <v>1</v>
+          </cell>
+          <cell r="F10" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G10" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="H10">
+            <v>100000</v>
+          </cell>
+          <cell r="I10">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>11</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="C11">
+            <v>5</v>
+          </cell>
+          <cell r="D11">
+            <v>20</v>
+          </cell>
+          <cell r="E11">
+            <v>1</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G11" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="H11">
+            <v>110000</v>
+          </cell>
+          <cell r="I11">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>12</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="C12">
+            <v>1</v>
+          </cell>
+          <cell r="D12">
+            <v>20</v>
+          </cell>
+          <cell r="E12">
+            <v>1</v>
+          </cell>
+          <cell r="F12" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G12" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="H12">
+            <v>120000</v>
+          </cell>
+          <cell r="I12">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>13</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="C13">
+            <v>2</v>
+          </cell>
+          <cell r="D13">
+            <v>20</v>
+          </cell>
+          <cell r="E13">
+            <v>1</v>
+          </cell>
+          <cell r="F13" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G13" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="H13">
+            <v>130000</v>
+          </cell>
+          <cell r="I13">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>14</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Eleaf iStick Pico (75 W) Authentic</v>
+          </cell>
+          <cell r="C14">
+            <v>3</v>
+          </cell>
+          <cell r="D14">
+            <v>20</v>
+          </cell>
+          <cell r="E14">
+            <v>1</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G14" t="str">
+            <v>Eleaf iStick Pico (75 W) Authentic</v>
+          </cell>
+          <cell r="H14">
+            <v>140000</v>
+          </cell>
+          <cell r="I14">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>15</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>Suorin Air</v>
+          </cell>
+          <cell r="C15">
+            <v>4</v>
+          </cell>
+          <cell r="D15">
+            <v>20</v>
+          </cell>
+          <cell r="E15">
+            <v>1</v>
+          </cell>
+          <cell r="F15" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G15" t="str">
+            <v>Suorin Air</v>
+          </cell>
+          <cell r="H15">
+            <v>150000</v>
+          </cell>
+          <cell r="I15">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>16</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>AugVape Druga Squonk</v>
+          </cell>
+          <cell r="C16">
+            <v>5</v>
+          </cell>
+          <cell r="D16">
+            <v>20</v>
+          </cell>
+          <cell r="E16">
+            <v>1</v>
+          </cell>
+          <cell r="F16" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G16" t="str">
+            <v>AugVape Druga Squonk</v>
+          </cell>
+          <cell r="H16">
+            <v>160000</v>
+          </cell>
+          <cell r="I16">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>17</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>Mecha Kit AV Timekeeper Revolver Kit</v>
+          </cell>
+          <cell r="C17">
+            <v>1</v>
+          </cell>
+          <cell r="D17">
+            <v>20</v>
+          </cell>
+          <cell r="E17">
+            <v>1</v>
+          </cell>
+          <cell r="F17" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G17" t="str">
+            <v>Mecha Kit AV Timekeeper Revolver Kit</v>
+          </cell>
+          <cell r="H17">
+            <v>170000</v>
+          </cell>
+          <cell r="I17">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>18</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>Smoant Charon TS (218 W)</v>
+          </cell>
+          <cell r="C18">
+            <v>2</v>
+          </cell>
+          <cell r="D18">
+            <v>20</v>
+          </cell>
+          <cell r="E18">
+            <v>1</v>
+          </cell>
+          <cell r="F18" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G18" t="str">
+            <v>Smoant Charon TS (218 W)</v>
+          </cell>
+          <cell r="H18">
+            <v>20000</v>
+          </cell>
+          <cell r="I18">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>19</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>GeekVape Aegis Legend</v>
+          </cell>
+          <cell r="C19">
+            <v>3</v>
+          </cell>
+          <cell r="D19">
+            <v>20</v>
+          </cell>
+          <cell r="E19">
+            <v>1</v>
+          </cell>
+          <cell r="F19" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G19" t="str">
+            <v>GeekVape Aegis Legend</v>
+          </cell>
+          <cell r="H19">
+            <v>180000</v>
+          </cell>
+          <cell r="I19">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>20</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>Voopoo Drag 2 Refresh Edition productnation</v>
+          </cell>
+          <cell r="C20">
+            <v>4</v>
+          </cell>
+          <cell r="D20">
+            <v>20</v>
+          </cell>
+          <cell r="E20">
+            <v>1</v>
+          </cell>
+          <cell r="F20" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G20" t="str">
+            <v>Voopoo Drag 2 Refresh Edition productnation</v>
+          </cell>
+          <cell r="H20">
+            <v>190000</v>
+          </cell>
+          <cell r="I20">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>21</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="C21">
+            <v>5</v>
+          </cell>
+          <cell r="D21">
+            <v>20</v>
+          </cell>
+          <cell r="E21">
+            <v>1</v>
+          </cell>
+          <cell r="F21" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G21" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="H21">
+            <v>200000</v>
+          </cell>
+          <cell r="I21">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>22</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="C22">
+            <v>1</v>
+          </cell>
+          <cell r="D22">
+            <v>20</v>
+          </cell>
+          <cell r="E22">
+            <v>1</v>
+          </cell>
+          <cell r="F22" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G22" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="H22">
+            <v>210000</v>
+          </cell>
+          <cell r="I22">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>23</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="C23">
+            <v>2</v>
+          </cell>
+          <cell r="D23">
+            <v>20</v>
+          </cell>
+          <cell r="E23">
+            <v>1</v>
+          </cell>
+          <cell r="F23" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G23" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="H23">
+            <v>220000</v>
+          </cell>
+          <cell r="I23">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>24</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="C24">
+            <v>3</v>
+          </cell>
+          <cell r="D24">
+            <v>20</v>
+          </cell>
+          <cell r="E24">
+            <v>1</v>
+          </cell>
+          <cell r="F24" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G24" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="H24">
+            <v>230000</v>
+          </cell>
+          <cell r="I24">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>25</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="C25">
+            <v>4</v>
+          </cell>
+          <cell r="D25">
+            <v>20</v>
+          </cell>
+          <cell r="E25">
+            <v>1</v>
+          </cell>
+          <cell r="F25" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G25" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="H25">
+            <v>240000</v>
+          </cell>
+          <cell r="I25">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>26</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="C26">
+            <v>5</v>
+          </cell>
+          <cell r="D26">
+            <v>20</v>
+          </cell>
+          <cell r="E26">
+            <v>1</v>
+          </cell>
+          <cell r="F26" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G26" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="H26">
+            <v>250000</v>
+          </cell>
+          <cell r="I26">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>27</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="C27">
+            <v>1</v>
+          </cell>
+          <cell r="D27">
+            <v>20</v>
+          </cell>
+          <cell r="E27">
+            <v>1</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G27" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="H27">
+            <v>260000</v>
+          </cell>
+          <cell r="I27">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>28</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="C28">
+            <v>2</v>
+          </cell>
+          <cell r="D28">
+            <v>20</v>
+          </cell>
+          <cell r="E28">
+            <v>1</v>
+          </cell>
+          <cell r="F28" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G28" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="H28">
+            <v>270000</v>
+          </cell>
+          <cell r="I28">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>29</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="C29">
+            <v>3</v>
+          </cell>
+          <cell r="D29">
+            <v>20</v>
+          </cell>
+          <cell r="E29">
+            <v>1</v>
+          </cell>
+          <cell r="F29" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G29" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="H29">
+            <v>280000</v>
+          </cell>
+          <cell r="I29">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>30</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="C30">
+            <v>4</v>
+          </cell>
+          <cell r="D30">
+            <v>20</v>
+          </cell>
+          <cell r="E30">
+            <v>1</v>
+          </cell>
+          <cell r="F30" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G30" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="H30">
+            <v>290000</v>
+          </cell>
+          <cell r="I30">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>31</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="C31">
+            <v>5</v>
+          </cell>
+          <cell r="D31">
+            <v>20</v>
+          </cell>
+          <cell r="E31">
+            <v>1</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="H31">
+            <v>300000</v>
+          </cell>
+          <cell r="I31">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>32</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="C32">
+            <v>1</v>
+          </cell>
+          <cell r="D32">
+            <v>20</v>
+          </cell>
+          <cell r="E32">
+            <v>1</v>
+          </cell>
+          <cell r="F32" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G32" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="H32">
+            <v>310000</v>
+          </cell>
+          <cell r="I32">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>33</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>Eleaf iStick Pico (75 W) Authentic</v>
+          </cell>
+          <cell r="C33">
+            <v>2</v>
+          </cell>
+          <cell r="D33">
+            <v>20</v>
+          </cell>
+          <cell r="E33">
+            <v>1</v>
+          </cell>
+          <cell r="F33" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G33" t="str">
+            <v>Eleaf iStick Pico (75 W) Authentic</v>
+          </cell>
+          <cell r="H33">
+            <v>320000</v>
+          </cell>
+          <cell r="I33">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>34</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>Suorin Air</v>
+          </cell>
+          <cell r="C34">
+            <v>3</v>
+          </cell>
+          <cell r="D34">
+            <v>20</v>
+          </cell>
+          <cell r="E34">
+            <v>1</v>
+          </cell>
+          <cell r="F34" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G34" t="str">
+            <v>Suorin Air</v>
+          </cell>
+          <cell r="H34">
+            <v>340000</v>
+          </cell>
+          <cell r="I34">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>35</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>AugVape Druga Squonk</v>
+          </cell>
+          <cell r="C35">
+            <v>4</v>
+          </cell>
+          <cell r="D35">
+            <v>20</v>
+          </cell>
+          <cell r="E35">
+            <v>1</v>
+          </cell>
+          <cell r="F35" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G35" t="str">
+            <v>AugVape Druga Squonk</v>
+          </cell>
+          <cell r="H35">
+            <v>350000</v>
+          </cell>
+          <cell r="I35">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>36</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>Mecha Kit AV Timekeeper Revolver Kit</v>
+          </cell>
+          <cell r="C36">
+            <v>5</v>
+          </cell>
+          <cell r="D36">
+            <v>20</v>
+          </cell>
+          <cell r="E36">
+            <v>1</v>
+          </cell>
+          <cell r="F36" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G36" t="str">
+            <v>Mecha Kit AV Timekeeper Revolver Kit</v>
+          </cell>
+          <cell r="H36">
+            <v>360000</v>
+          </cell>
+          <cell r="I36">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>37</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>Smoant Charon TS (218 W)</v>
+          </cell>
+          <cell r="C37">
+            <v>1</v>
+          </cell>
+          <cell r="D37">
+            <v>20</v>
+          </cell>
+          <cell r="E37">
+            <v>1</v>
+          </cell>
+          <cell r="F37" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G37" t="str">
+            <v>Smoant Charon TS (218 W)</v>
+          </cell>
+          <cell r="H37">
+            <v>370000</v>
+          </cell>
+          <cell r="I37">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>38</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>GeekVape Aegis Legend</v>
+          </cell>
+          <cell r="C38">
+            <v>2</v>
+          </cell>
+          <cell r="D38">
+            <v>20</v>
+          </cell>
+          <cell r="E38">
+            <v>1</v>
+          </cell>
+          <cell r="F38" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G38" t="str">
+            <v>GeekVape Aegis Legend</v>
+          </cell>
+          <cell r="H38">
+            <v>380000</v>
+          </cell>
+          <cell r="I38">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>39</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>Voopoo Drag 2 Refresh Edition productnation</v>
+          </cell>
+          <cell r="C39">
+            <v>3</v>
+          </cell>
+          <cell r="D39">
+            <v>20</v>
+          </cell>
+          <cell r="E39">
+            <v>1</v>
+          </cell>
+          <cell r="F39" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G39" t="str">
+            <v>Voopoo Drag 2 Refresh Edition productnation</v>
+          </cell>
+          <cell r="H39">
+            <v>380000</v>
+          </cell>
+          <cell r="I39">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>40</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="C40">
+            <v>4</v>
+          </cell>
+          <cell r="D40">
+            <v>20</v>
+          </cell>
+          <cell r="E40">
+            <v>1</v>
+          </cell>
+          <cell r="F40" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G40" t="str">
+            <v>Dovpo MVV 2 Panda Edition</v>
+          </cell>
+          <cell r="H40">
+            <v>390000</v>
+          </cell>
+          <cell r="I40">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>41</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="C41">
+            <v>5</v>
+          </cell>
+          <cell r="D41">
+            <v>20</v>
+          </cell>
+          <cell r="E41">
+            <v>1</v>
+          </cell>
+          <cell r="F41" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G41" t="str">
+            <v>Joyetech Exceed Grip</v>
+          </cell>
+          <cell r="H41">
+            <v>400000</v>
+          </cell>
+          <cell r="I41">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>42</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="C42">
+            <v>1</v>
+          </cell>
+          <cell r="D42">
+            <v>20</v>
+          </cell>
+          <cell r="E42">
+            <v>1</v>
+          </cell>
+          <cell r="F42" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G42" t="str">
+            <v>Upods Cube</v>
+          </cell>
+          <cell r="H42">
+            <v>410000</v>
+          </cell>
+          <cell r="I42">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>43</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="C43">
+            <v>2</v>
+          </cell>
+          <cell r="D43">
+            <v>20</v>
+          </cell>
+          <cell r="E43">
+            <v>1</v>
+          </cell>
+          <cell r="F43" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G43" t="str">
+            <v>Vaporite Mecha Kit 22mm</v>
+          </cell>
+          <cell r="H43">
+            <v>420000</v>
+          </cell>
+          <cell r="I43">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>44</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="C44">
+            <v>3</v>
+          </cell>
+          <cell r="D44">
+            <v>20</v>
+          </cell>
+          <cell r="E44">
+            <v>1</v>
+          </cell>
+          <cell r="F44" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G44" t="str">
+            <v>HexOhm v3.0 30 Amp Anodized by Craving Vapor</v>
+          </cell>
+          <cell r="H44">
+            <v>430000</v>
+          </cell>
+          <cell r="I44">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>45</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="C45">
+            <v>4</v>
+          </cell>
+          <cell r="D45">
+            <v>20</v>
+          </cell>
+          <cell r="E45">
+            <v>1</v>
+          </cell>
+          <cell r="F45" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G45" t="str">
+            <v>JUUL</v>
+          </cell>
+          <cell r="H45">
+            <v>440000</v>
+          </cell>
+          <cell r="I45">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>46</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="C46">
+            <v>5</v>
+          </cell>
+          <cell r="D46">
+            <v>20</v>
+          </cell>
+          <cell r="E46">
+            <v>1</v>
+          </cell>
+          <cell r="F46" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G46" t="str">
+            <v>SMOK Fetch Mini</v>
+          </cell>
+          <cell r="H46">
+            <v>450000</v>
+          </cell>
+          <cell r="I46">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>47</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="C47">
+            <v>1</v>
+          </cell>
+          <cell r="D47">
+            <v>20</v>
+          </cell>
+          <cell r="E47">
+            <v>1</v>
+          </cell>
+          <cell r="F47" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G47" t="str">
+            <v>Art Mod by Preva x Owlexandrea</v>
+          </cell>
+          <cell r="H47">
+            <v>460000</v>
+          </cell>
+          <cell r="I47">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>48</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="C48">
+            <v>2</v>
+          </cell>
+          <cell r="D48">
+            <v>20</v>
+          </cell>
+          <cell r="E48">
+            <v>1</v>
+          </cell>
+          <cell r="F48" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G48" t="str">
+            <v>Joyetech Teros Zoo Pod</v>
+          </cell>
+          <cell r="H48">
+            <v>470000</v>
+          </cell>
+          <cell r="I48">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>49</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="C49">
+            <v>3</v>
+          </cell>
+          <cell r="D49">
+            <v>20</v>
+          </cell>
+          <cell r="E49">
+            <v>1</v>
+          </cell>
+          <cell r="F49" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G49" t="str">
+            <v>Uwell Caliburn</v>
+          </cell>
+          <cell r="H49">
+            <v>480000</v>
+          </cell>
+          <cell r="I49">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>50</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="C50">
+            <v>4</v>
+          </cell>
+          <cell r="D50">
+            <v>20</v>
+          </cell>
+          <cell r="E50">
+            <v>1</v>
+          </cell>
+          <cell r="F50" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G50" t="str">
+            <v>Teslacigs Terminator VAPE</v>
+          </cell>
+          <cell r="H50">
+            <v>490000</v>
+          </cell>
+          <cell r="I50">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>51</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="C51">
+            <v>5</v>
+          </cell>
+          <cell r="D51">
+            <v>20</v>
+          </cell>
+          <cell r="E51">
+            <v>1</v>
+          </cell>
+          <cell r="F51" t="str">
+            <v>Vapor Terbaik</v>
+          </cell>
+          <cell r="G51" t="str">
+            <v>Smok RPM 40</v>
+          </cell>
+          <cell r="H51">
+            <v>500000</v>
+          </cell>
+          <cell r="I51">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>53</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>ervan</v>
+          </cell>
+          <cell r="C52">
+            <v>2</v>
+          </cell>
+          <cell r="D52">
+            <v>200</v>
+          </cell>
+          <cell r="E52">
+            <v>0</v>
+          </cell>
+          <cell r="F52" t="str">
+            <v>200                                 </v>
+          </cell>
+          <cell r="G52" t="str">
+            <v>2022-07-17JANE.png</v>
+          </cell>
+          <cell r="H52">
+            <v>200</v>
+          </cell>
+          <cell r="I52">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3938,7 +5544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -4306,6 +5912,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4880,12 +6498,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:I20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5377,4 +6995,335 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="O11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="16">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16">
+        <v>4</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="G12" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" t="s">
+        <v>143</v>
+      </c>
+      <c r="J12" t="s">
+        <v>142</v>
+      </c>
+      <c r="K12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12" t="str">
+        <f>"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;"',"&amp;M13&amp;"),"</f>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (1,31,2,1,20000',1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="16">
+        <v>3</v>
+      </c>
+      <c r="C13" s="16">
+        <v>4</v>
+      </c>
+      <c r="D13" s="16">
+        <v>5</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>31</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f>VLOOKUP(J13,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" ref="O13:O15" si="0">"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;"',"&amp;M14&amp;"),"</f>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (2,31,3,1,30000',1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="16">
+        <v>5</v>
+      </c>
+      <c r="C14" s="16">
+        <v>6</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>31</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>VLOOKUP(J14,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>30000</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (3,31,4,1,40000',1),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="16">
+        <v>2</v>
+      </c>
+      <c r="C15" s="16">
+        <v>3</v>
+      </c>
+      <c r="D15" s="16">
+        <v>5</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>31</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f>VLOOKUP(J15,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>40000</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (,,,,',),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2</v>
+      </c>
+      <c r="C17" s="16">
+        <v>3</v>
+      </c>
+      <c r="D17" s="16">
+        <v>4</v>
+      </c>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2022 08 06 04:55
</commit_message>
<xml_diff>
--- a/assets/apriori baru.xlsx
+++ b/assets/apriori baru.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="contoh 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="162">
   <si>
     <t>Data</t>
   </si>
@@ -475,6 +475,48 @@
   </si>
   <si>
     <t>keranjang1</t>
+  </si>
+  <si>
+    <t>keranjang</t>
+  </si>
+  <si>
+    <t>INSERT INTO `checkout`(`id_checkout`, `tanggal_transaksi`, `tanggal_kadaluarsa`, `status_transaksi`, `jumlah_checkout`, `id_keranjang`, `id_user`) VALUES ('[value-1]','[value-2]','[value-3]','[value-4]','[value-5]','[value-6]','[value-7]')</t>
+  </si>
+  <si>
+    <t>2022-08-01</t>
+  </si>
+  <si>
+    <t>2022-08-02</t>
+  </si>
+  <si>
+    <t>2022-08-03</t>
+  </si>
+  <si>
+    <t>2022-08-04</t>
+  </si>
+  <si>
+    <t>2022-08-05</t>
+  </si>
+  <si>
+    <t>2022-08-06</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
+  </si>
+  <si>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>9,10,11</t>
+  </si>
+  <si>
+    <t>12,13,14,15</t>
+  </si>
+  <si>
+    <t>16,17,18,19</t>
   </si>
 </sst>
 </file>
@@ -509,7 +551,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,6 +573,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -728,6 +800,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,16 +813,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5544,8 +5622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5637,10 +5715,10 @@
       <c r="J13" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="22"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -5828,10 +5906,10 @@
       <c r="J29" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="L29" s="24"/>
+      <c r="L29" s="26"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -5937,13 +6015,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -6999,10 +7077,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O17"/>
+  <dimension ref="A2:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7011,7 +7089,7 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -7027,82 +7105,82 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="27" t="s">
@@ -7118,16 +7196,16 @@
       <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="24"/>
       <c r="O11" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="23" t="s">
         <v>132</v>
       </c>
       <c r="B12" s="16">
@@ -7140,9 +7218,6 @@
         <v>4</v>
       </c>
       <c r="E12" s="16"/>
-      <c r="G12" s="28" t="s">
-        <v>147</v>
-      </c>
       <c r="H12" t="s">
         <v>141</v>
       </c>
@@ -7162,12 +7237,12 @@
         <v>146</v>
       </c>
       <c r="O12" t="str">
-        <f>"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;"',"&amp;M13&amp;"),"</f>
-        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (1,31,2,1,20000',1),</v>
+        <f>"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;","&amp;M13&amp;"),"</f>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (1,31,2,1,20000,1),</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="29" t="s">
         <v>133</v>
       </c>
       <c r="B13" s="16">
@@ -7180,13 +7255,16 @@
         <v>5</v>
       </c>
       <c r="E13" s="16"/>
+      <c r="G13" s="23" t="s">
+        <v>147</v>
+      </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
         <v>31</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="23">
         <v>2</v>
       </c>
       <c r="K13">
@@ -7200,12 +7278,12 @@
         <v>1</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" ref="O13:O15" si="0">"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;"',"&amp;M14&amp;"),"</f>
-        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (2,31,3,1,30000',1),</v>
+        <f>"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;","&amp;M13&amp;"),"</f>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (1,31,2,1,20000,1),</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="30" t="s">
         <v>134</v>
       </c>
       <c r="B14" s="16">
@@ -7222,7 +7300,7 @@
       <c r="I14">
         <v>31</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="23">
         <v>3</v>
       </c>
       <c r="K14">
@@ -7236,12 +7314,12 @@
         <v>1</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (3,31,4,1,40000',1),</v>
+        <f t="shared" ref="O14:O38" si="0">"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;"),"</f>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (2,31,3,1,30000,1),</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="31" t="s">
         <v>135</v>
       </c>
       <c r="B15" s="16">
@@ -7260,7 +7338,7 @@
       <c r="I15">
         <v>31</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="23">
         <v>4</v>
       </c>
       <c r="K15">
@@ -7275,11 +7353,11 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (,,,,',),</v>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (3,31,4,1,40000,1),</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="32" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="16">
@@ -7294,9 +7372,35 @@
       <c r="E16" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G16" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>31</v>
+      </c>
+      <c r="J16" s="29">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f>VLOOKUP(J16,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>30000</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (4,31,3,1,30000,1),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>137</v>
       </c>
       <c r="B17" s="16">
@@ -7310,6 +7414,576 @@
       </c>
       <c r="E17" s="16">
         <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+      <c r="J17" s="29">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f>VLOOKUP(J17,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>40000</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (5,31,4,1,40000,1),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>31</v>
+      </c>
+      <c r="J18" s="29">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f>VLOOKUP(J18,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>50000</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (6,31,5,1,50000,1),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G19" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>31</v>
+      </c>
+      <c r="J19" s="30">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f>VLOOKUP(J19,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>50000</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (7,31,5,1,50000,1),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>31</v>
+      </c>
+      <c r="J20" s="30">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f>VLOOKUP(J20,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>60000</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (8,31,6,1,60000,1),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G21" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21">
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <v>31</v>
+      </c>
+      <c r="J21" s="31">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f>VLOOKUP(J21,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (9,31,2,1,20000,1),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>31</v>
+      </c>
+      <c r="J22" s="31">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f>VLOOKUP(J22,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>30000</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (10,31,3,1,30000,1),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>31</v>
+      </c>
+      <c r="J23" s="31">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f>VLOOKUP(J23,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>50000</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (11,31,5,1,50000,1),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G24" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24">
+        <v>12</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
+      </c>
+      <c r="J24" s="32">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f>VLOOKUP(J24,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (12,31,2,1,20000,1),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <v>31</v>
+      </c>
+      <c r="J25" s="32">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <f>VLOOKUP(J25,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>30000</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (13,31,3,1,30000,1),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <v>31</v>
+      </c>
+      <c r="J26" s="32">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f>VLOOKUP(J26,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>40000</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (14,31,4,1,40000,1),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27">
+        <v>31</v>
+      </c>
+      <c r="J27" s="32">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f>VLOOKUP(J27,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>60000</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (15,31,6,1,60000,1),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G28" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>31</v>
+      </c>
+      <c r="J28" s="33">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f>VLOOKUP(J28,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (16,31,2,1,20000,1),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>17</v>
+      </c>
+      <c r="I29">
+        <v>31</v>
+      </c>
+      <c r="J29" s="33">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <f>VLOOKUP(J29,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>30000</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (17,31,3,1,30000,1),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>18</v>
+      </c>
+      <c r="I30">
+        <v>31</v>
+      </c>
+      <c r="J30" s="33">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <f>VLOOKUP(J30,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>40000</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (18,31,4,1,40000,1),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>19</v>
+      </c>
+      <c r="I31">
+        <v>31</v>
+      </c>
+      <c r="J31" s="33">
+        <v>5</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <f>VLOOKUP(J31,[1]produk!A$2:I$52,8,FALSE)</f>
+        <v>50000</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (19,31,5,1,50000,1),</v>
+      </c>
+    </row>
+    <row r="37" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G38" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>90000</v>
+      </c>
+      <c r="M38" t="s">
+        <v>156</v>
+      </c>
+      <c r="N38">
+        <v>31</v>
+      </c>
+      <c r="O38" t="str">
+        <f>" ("&amp;H38&amp;",'"&amp;I38&amp;"','"&amp;J38&amp;"',"&amp;K38&amp;","&amp;L38&amp;",'"&amp;M38&amp;"', "&amp;N38&amp;"),"</f>
+        <v xml:space="preserve"> (1,'2022-08-01','2022-08-01',1,90000,'1,2,3', 31),</v>
+      </c>
+    </row>
+    <row r="39" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G39" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>120000</v>
+      </c>
+      <c r="M39" t="s">
+        <v>157</v>
+      </c>
+      <c r="N39">
+        <v>31</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" ref="O39:O43" si="1">" ("&amp;H39&amp;",'"&amp;I39&amp;"','"&amp;J39&amp;"',"&amp;K39&amp;","&amp;L39&amp;",'"&amp;M39&amp;"', "&amp;N39&amp;"),"</f>
+        <v xml:space="preserve"> (2,'2022-08-02','2022-08-02',1,120000,'4,5,6', 31),</v>
+      </c>
+    </row>
+    <row r="40" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G40" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="J40" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>110000</v>
+      </c>
+      <c r="M40" t="s">
+        <v>158</v>
+      </c>
+      <c r="N40">
+        <v>31</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> (3,'2022-08-03','2022-08-03',1,110000,'7,8', 31),</v>
+      </c>
+    </row>
+    <row r="41" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G41" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>100000</v>
+      </c>
+      <c r="M41" t="s">
+        <v>159</v>
+      </c>
+      <c r="N41">
+        <v>31</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> (4,'2022-08-04','2022-08-04',1,100000,'9,10,11', 31),</v>
+      </c>
+    </row>
+    <row r="42" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G42" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>150000</v>
+      </c>
+      <c r="M42" t="s">
+        <v>160</v>
+      </c>
+      <c r="N42">
+        <v>31</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> (5,'2022-08-05','2022-08-05',1,150000,'12,13,14,15', 31),</v>
+      </c>
+    </row>
+    <row r="43" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G43" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43">
+        <v>6</v>
+      </c>
+      <c r="I43" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>140000</v>
+      </c>
+      <c r="M43" t="s">
+        <v>161</v>
+      </c>
+      <c r="N43">
+        <v>31</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> (6,'2022-08-06','2022-08-06',1,140000,'16,17,18,19', 31),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022 08 06 04:550
</commit_message>
<xml_diff>
--- a/assets/apriori baru.xlsx
+++ b/assets/apriori baru.xlsx
@@ -551,7 +551,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +603,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,6 +816,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,12 +837,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5622,8 +5642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5715,10 +5735,10 @@
       <c r="J13" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="30"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -5734,6 +5754,10 @@
         <f>SUM(K18/L18*100)</f>
         <v>75</v>
       </c>
+      <c r="L14">
+        <f>K14/100</f>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -5749,6 +5773,10 @@
         <f>SUM(K19/L19*100)</f>
         <v>100</v>
       </c>
+      <c r="L15">
+        <f t="shared" ref="L15:L16" si="0">K15/100</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -5764,6 +5792,10 @@
         <f>SUM(K20/L20*100)</f>
         <v>75</v>
       </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -5783,10 +5815,10 @@
       <c r="J18" t="s">
         <v>117</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="36">
         <v>3</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="37">
         <v>4</v>
       </c>
     </row>
@@ -5794,10 +5826,10 @@
       <c r="J19" t="s">
         <v>116</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="36">
         <v>3</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="37">
         <v>3</v>
       </c>
     </row>
@@ -5808,10 +5840,10 @@
       <c r="J20" t="s">
         <v>118</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="36">
         <v>3</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="37">
         <v>4</v>
       </c>
     </row>
@@ -5830,11 +5862,11 @@
       <c r="A22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="38">
         <v>4</v>
       </c>
       <c r="C22" s="8">
-        <f>SUM(4/6*100)</f>
+        <f>SUM(B22/6*100)</f>
         <v>66.666666666666657</v>
       </c>
       <c r="J22" t="s">
@@ -5845,11 +5877,11 @@
       <c r="A23" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="38">
         <v>3</v>
       </c>
       <c r="C23" s="8">
-        <f>SUM(3/6*100)</f>
+        <f>SUM(B23/6*100)</f>
         <v>50</v>
       </c>
     </row>
@@ -5860,17 +5892,20 @@
       <c r="B24" s="6">
         <v>2</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="8">
+        <f t="shared" ref="C24:C27" si="1">SUM(B24/6*100)</f>
+        <v>33.333333333333329</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="38">
         <v>4</v>
       </c>
       <c r="C25" s="8">
-        <f>SUM(4/6*100)</f>
+        <f t="shared" si="1"/>
         <v>66.666666666666657</v>
       </c>
     </row>
@@ -5882,7 +5917,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="8">
-        <f>SUM(3/6*100)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -5893,7 +5928,10 @@
       <c r="B27" s="6">
         <v>2</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="8">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
@@ -5906,10 +5944,10 @@
       <c r="J29" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="K29" s="25" t="s">
+      <c r="K29" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="L29" s="26"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -5930,10 +5968,10 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="35">
         <v>3</v>
       </c>
       <c r="C31" s="8">
@@ -6015,13 +6053,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -7079,8 +7117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7105,101 +7143,101 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="30"/>
       <c r="O11" t="s">
         <v>139</v>
       </c>
@@ -7242,7 +7280,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="24" t="s">
         <v>133</v>
       </c>
       <c r="B13" s="16">
@@ -7283,7 +7321,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>134</v>
       </c>
       <c r="B14" s="16">
@@ -7314,12 +7352,12 @@
         <v>1</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" ref="O14:O38" si="0">"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;"),"</f>
+        <f t="shared" ref="O14:O31" si="0">"INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES ("&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;"),"</f>
         <v>INSERT INTO `keranjang`(`id_keranjang`, `id_user`, `id_produk`, `jumlah_keranjang`, `harga_keranjang`, `status_keranjang`) VALUES (2,31,3,1,30000,1),</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="26" t="s">
         <v>135</v>
       </c>
       <c r="B15" s="16">
@@ -7357,7 +7395,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="27" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="16">
@@ -7372,7 +7410,7 @@
       <c r="E16" s="16">
         <v>6</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="24" t="s">
         <v>148</v>
       </c>
       <c r="H16">
@@ -7381,7 +7419,7 @@
       <c r="I16">
         <v>31</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="24">
         <v>3</v>
       </c>
       <c r="K16">
@@ -7400,7 +7438,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="28" t="s">
         <v>137</v>
       </c>
       <c r="B17" s="16">
@@ -7421,7 +7459,7 @@
       <c r="I17">
         <v>31</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="24">
         <v>4</v>
       </c>
       <c r="K17">
@@ -7446,7 +7484,7 @@
       <c r="I18">
         <v>31</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="24">
         <v>5</v>
       </c>
       <c r="K18">
@@ -7465,7 +7503,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="25" t="s">
         <v>148</v>
       </c>
       <c r="H19">
@@ -7474,7 +7512,7 @@
       <c r="I19">
         <v>31</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="25">
         <v>5</v>
       </c>
       <c r="K19">
@@ -7499,7 +7537,7 @@
       <c r="I20">
         <v>31</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="25">
         <v>6</v>
       </c>
       <c r="K20">
@@ -7518,7 +7556,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="26" t="s">
         <v>148</v>
       </c>
       <c r="H21">
@@ -7527,7 +7565,7 @@
       <c r="I21">
         <v>31</v>
       </c>
-      <c r="J21" s="31">
+      <c r="J21" s="26">
         <v>2</v>
       </c>
       <c r="K21">
@@ -7552,7 +7590,7 @@
       <c r="I22">
         <v>31</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="26">
         <v>3</v>
       </c>
       <c r="K22">
@@ -7577,7 +7615,7 @@
       <c r="I23">
         <v>31</v>
       </c>
-      <c r="J23" s="31">
+      <c r="J23" s="26">
         <v>5</v>
       </c>
       <c r="K23">
@@ -7596,7 +7634,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="27" t="s">
         <v>148</v>
       </c>
       <c r="H24">
@@ -7605,7 +7643,7 @@
       <c r="I24">
         <v>31</v>
       </c>
-      <c r="J24" s="32">
+      <c r="J24" s="27">
         <v>2</v>
       </c>
       <c r="K24">
@@ -7630,7 +7668,7 @@
       <c r="I25">
         <v>31</v>
       </c>
-      <c r="J25" s="32">
+      <c r="J25" s="27">
         <v>3</v>
       </c>
       <c r="K25">
@@ -7655,7 +7693,7 @@
       <c r="I26">
         <v>31</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="27">
         <v>4</v>
       </c>
       <c r="K26">
@@ -7680,7 +7718,7 @@
       <c r="I27">
         <v>31</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="27">
         <v>6</v>
       </c>
       <c r="K27">
@@ -7699,7 +7737,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="28" t="s">
         <v>148</v>
       </c>
       <c r="H28">
@@ -7708,7 +7746,7 @@
       <c r="I28">
         <v>31</v>
       </c>
-      <c r="J28" s="33">
+      <c r="J28" s="28">
         <v>2</v>
       </c>
       <c r="K28">
@@ -7733,7 +7771,7 @@
       <c r="I29">
         <v>31</v>
       </c>
-      <c r="J29" s="33">
+      <c r="J29" s="28">
         <v>3</v>
       </c>
       <c r="K29">
@@ -7758,7 +7796,7 @@
       <c r="I30">
         <v>31</v>
       </c>
-      <c r="J30" s="33">
+      <c r="J30" s="28">
         <v>4</v>
       </c>
       <c r="K30">
@@ -7783,7 +7821,7 @@
       <c r="I31">
         <v>31</v>
       </c>
-      <c r="J31" s="33">
+      <c r="J31" s="28">
         <v>5</v>
       </c>
       <c r="K31">
@@ -7813,10 +7851,10 @@
       <c r="H38">
         <v>1</v>
       </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="29" t="s">
         <v>150</v>
       </c>
       <c r="K38">
@@ -7837,16 +7875,16 @@
       </c>
     </row>
     <row r="39" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="24" t="s">
         <v>133</v>
       </c>
       <c r="H39">
         <v>2</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="J39" s="34" t="s">
+      <c r="J39" s="29" t="s">
         <v>151</v>
       </c>
       <c r="K39">
@@ -7867,16 +7905,16 @@
       </c>
     </row>
     <row r="40" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="25" t="s">
         <v>134</v>
       </c>
       <c r="H40">
         <v>3</v>
       </c>
-      <c r="I40" s="34" t="s">
+      <c r="I40" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="J40" s="34" t="s">
+      <c r="J40" s="29" t="s">
         <v>152</v>
       </c>
       <c r="K40">
@@ -7897,16 +7935,16 @@
       </c>
     </row>
     <row r="41" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="26" t="s">
         <v>135</v>
       </c>
       <c r="H41">
         <v>4</v>
       </c>
-      <c r="I41" s="34" t="s">
+      <c r="I41" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J41" s="34" t="s">
+      <c r="J41" s="29" t="s">
         <v>153</v>
       </c>
       <c r="K41">
@@ -7927,16 +7965,16 @@
       </c>
     </row>
     <row r="42" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G42" s="32" t="s">
+      <c r="G42" s="27" t="s">
         <v>136</v>
       </c>
       <c r="H42">
         <v>5</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="J42" s="34" t="s">
+      <c r="J42" s="29" t="s">
         <v>154</v>
       </c>
       <c r="K42">
@@ -7957,16 +7995,16 @@
       </c>
     </row>
     <row r="43" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G43" s="33" t="s">
+      <c r="G43" s="28" t="s">
         <v>137</v>
       </c>
       <c r="H43">
         <v>6</v>
       </c>
-      <c r="I43" s="34" t="s">
+      <c r="I43" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="J43" s="34" t="s">
+      <c r="J43" s="29" t="s">
         <v>155</v>
       </c>
       <c r="K43">

</xml_diff>